<commit_message>
Code Version 2018/4/6, Ettrore_icf_sc 1.3 update - psudo-BCS
</commit_message>
<xml_diff>
--- a/Fortran code/Fortran_bcs_pin_ettore/Record/Record1.2.xlsx
+++ b/Fortran code/Fortran_bcs_pin_ettore/Record/Record1.2.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:400001_{C89CAA0E-83F6-43D5-87C5-1DBFCCD9FD2A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{33CD6CF5-BD2E-4074-A73C-3A7F74349DB4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43:E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>